<commit_message>
Choose Your Medicine 업데이트
전체 새로 한글화
(오타수정)
</commit_message>
<xml_diff>
--- a/Pull Request Here/Choose Your Medicine - 2937201140/Choose Your Medicine - 2937201140.xlsx
+++ b/Pull Request Here/Choose Your Medicine - 2937201140/Choose Your Medicine - 2937201140.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PDSSO2\Desktop\RimworldExtractor-Standard\RIM EXCEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC552C1-85B7-4410-A8F7-89B491AD18CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{079D7DB2-A2A1-4F3F-BEEF-59B33F268636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -558,10 +558,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>목록의 모든 항목을 복사한 항목으로 교체합니다. 정말로 그렇게 하시겠습니까?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>모든 페이지</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -794,10 +790,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>모든 페이지를 기본 설정으로 되돌리시겠습니까?\n\n모드 추가나 게임 업데이트로 새로운 질병/부상이 등장하면 추가하고, 더미데이터는 삭제합니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>{0}개의 더미데이터를 삭제했고, {1}개의 질병/부상을 추가했습니다. 로그에서 세부사항을 확인할 수 있습니다.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -894,18 +886,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>환자가 위험하면 응급 치료를 진행합니다.\n\n[항체 형성] &lt; [진행도+설정값]\n\n예: [항체 50%], [진행 45%]이라면,\n설정값은 5%~100% 사이에 있어야\n응급 치료를 진행합니다.\n\n해당하지 않으면 의사는 [단순 치료]를 검토합니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>환자가 안전하면 단순 치료를 진행합니다.\n\n[항체 형성] &gt; [진행도+설정값]\n\n예: [항체 80%], [진행 54.9%]이라면,\n설정값은 0%~25% 사이에 있어야\n단순 치료를 진행합니다.\n\n해당하지 않으면 의사는 [일반 치료]를 검토합니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>항체와 관련 없는 증상은 일반 치료로 진행합니다.\n\n참고: 항체와 관련한 질병이라면,\n"초기-&gt;응급-&gt;단순-&gt;일반" 순으로 검토해보며 진행합니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>《2》 초기 치료 :\n항체가 [초기 치료]보다 낮으면,\n지정한 의약품을 최대로 사용합니다.\n\n항체가 19.9%이고, [초기 치료]를 20%~100% 사이로 했다면, 의사는 초기 치료를 진행합니다.\n\n해당하지 않으면 《3》으로 진행합니다.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -914,10 +894,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>《4》 단순 치료 :\n항체가 [진행도+단순 치료]보다 높으면,\n설정한 의약품을 최대로 사용합니다.\n\n항체가 80%이고 진행도가 54.9%이며,\n[단순 치료]을 0%~25% 사이로 했다면, 의사는 단순 치료를 진행합니다.\n\n해당하지 않으면 《5》로 진행합니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>규칙 순서\n《1》 강제 지정:\n먼저, 플레이어가 건강 탭에서 환자의 증상마다 치료를 강제로 지정했는지를 확인합니다.\n\n건강 탭에서 증상의 상세정보(i) 바로 왼쪽에 위치한 흐릿한 박스를 클릭하면 사용할 최대 의약품을 강제로 지정할 수 있습니다.\n\n강제로 지정했다면, 모든 정책을 무시하고 선택한 대로 치료합니다.\n\n지정하지 않았다면, 현재 정책을 적용하기 위해 《2》로 진행합니다.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -926,10 +902,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>질병이 발생하면 초기 치료를 진행합니다.\n\n[항체 형성] &lt; [설정값]\n\n예: [항체 19.9%]이라면,\n설정값은 20%~100% 사이에 있어야\n초기 치료를 진행합니다.\n\n해당하지 않으면 의사는 [응급 치료]를 검토합니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>단순 치료 (질병)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -939,6 +911,34 @@
   </si>
   <si>
     <t>초기 치료 (질병)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>항체와 관련 없는 증상은 일반 치료로 진행합니다.\n\n참고: 항체와 관련한 질병이면,\n"초기-&gt;응급-&gt;단순-&gt;일반" 순으로 검토해보며 진행합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>환자가 안전하면 단순 치료를 진행합니다.\n\n[항체 형성] &gt; [진행도+설정값]\n\n예: [항체 80%], [진행 54.9%]일 땐,\n설정값은 0%~25% 사이에 있어야\n단순 치료를 진행합니다.\n\n해당하지 않으면 의사는 [일반 치료]를 검토합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>환자가 위험하면 응급 치료를 진행합니다.\n\n[항체 형성] &lt; [진행도+설정값]\n\n예: [항체 50%], [진행 45%]일 땐,\n설정값은 5%~100% 사이에 있어야\n응급 치료를 진행합니다.\n\n해당하지 않으면 의사는 [단순 치료]를 검토합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>질병이 발생하면 초기 치료를 진행합니다.\n\n[항체 형성] &lt; [설정값]\n\n예: [항체 19.9%]일 땐,\n설정값은 20%~100% 사이에 있어야\n초기 치료를 진행합니다.\n\n해당하지 않으면 의사는 [응급 치료]를 검토합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>《4》 단순 치료 :\n항체가 [진행도+단순 치료]보다 높으면,\n설정한 의약품을 최대로 사용합니다.\n\n항체가 80%이고 진행도가 54.9%이며,\n[단순 치료]를 0%~25% 사이로 했다면, 의사는 단순 치료를 진행합니다.\n\n해당하지 않으면 《5》로 진행합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>모든 페이지를 기본 설정으로 되돌리시겠습니까?\n\n참고: [수술 의약품 관리] 설정도 기본 설정으로 되돌아갑니다.\n\n모드 추가나 게임 업데이트로 새로운 질병/부상이 등장하면 추가하고, 더미데이터는 삭제합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>목록의 항목들을 복사한 항목들로 교체합니다. 정말로 그렇게 하시겠습니까?</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1348,7 +1348,7 @@
         <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1365,7 +1365,7 @@
         <v>176</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1382,7 +1382,7 @@
         <v>177</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>178</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1399,7 +1399,7 @@
         <v>17</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1416,7 +1416,7 @@
         <v>20</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1430,10 +1430,10 @@
         <v>22</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -1447,10 +1447,10 @@
         <v>24</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>237</v>
+        <v>272</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1464,10 +1464,10 @@
         <v>26</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1481,10 +1481,10 @@
         <v>28</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -1498,10 +1498,10 @@
         <v>30</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1515,10 +1515,10 @@
         <v>32</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1532,10 +1532,10 @@
         <v>34</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1549,10 +1549,10 @@
         <v>36</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>262</v>
+        <v>269</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1566,10 +1566,10 @@
         <v>38</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1583,7 +1583,7 @@
         <v>40</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>270</v>
@@ -1603,7 +1603,7 @@
         <v>43</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1620,7 +1620,7 @@
         <v>46</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1637,7 +1637,7 @@
         <v>49</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1654,7 +1654,7 @@
         <v>52</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -1668,10 +1668,10 @@
         <v>54</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -1685,10 +1685,10 @@
         <v>56</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1702,10 +1702,10 @@
         <v>58</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1722,7 +1722,7 @@
         <v>61</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1739,7 +1739,7 @@
         <v>64</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1756,7 +1756,7 @@
         <v>67</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1770,10 +1770,10 @@
         <v>69</v>
       </c>
       <c r="E27" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1790,7 +1790,7 @@
         <v>72</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1804,10 +1804,10 @@
         <v>74</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1824,7 +1824,7 @@
         <v>77</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1841,7 +1841,7 @@
         <v>80</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1858,7 +1858,7 @@
         <v>83</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1875,7 +1875,7 @@
         <v>86</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1892,7 +1892,7 @@
         <v>89</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1909,7 +1909,7 @@
         <v>92</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1926,7 +1926,7 @@
         <v>95</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1943,7 +1943,7 @@
         <v>98</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1960,7 +1960,7 @@
         <v>101</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1977,7 +1977,7 @@
         <v>104</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1988,13 +1988,13 @@
         <v>13</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -2011,7 +2011,7 @@
         <v>108</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -2028,7 +2028,7 @@
         <v>111</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -2045,7 +2045,7 @@
         <v>114</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -2062,7 +2062,7 @@
         <v>117</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -2076,10 +2076,10 @@
         <v>119</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -2093,10 +2093,10 @@
         <v>121</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -2110,10 +2110,10 @@
         <v>123</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -2127,10 +2127,10 @@
         <v>125</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -2147,7 +2147,7 @@
         <v>128</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -2164,7 +2164,7 @@
         <v>131</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -2181,7 +2181,7 @@
         <v>134</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -2198,7 +2198,7 @@
         <v>137</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -2212,10 +2212,10 @@
         <v>139</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -2232,7 +2232,7 @@
         <v>142</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -2249,7 +2249,7 @@
         <v>145</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -2263,10 +2263,10 @@
         <v>147</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -2280,10 +2280,10 @@
         <v>149</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -2300,7 +2300,7 @@
         <v>152</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -2314,10 +2314,10 @@
         <v>154</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -2334,7 +2334,7 @@
         <v>157</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -2348,10 +2348,10 @@
         <v>159</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -2365,10 +2365,10 @@
         <v>161</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -2382,10 +2382,10 @@
         <v>163</v>
       </c>
       <c r="E63" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F63" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -2399,10 +2399,10 @@
         <v>165</v>
       </c>
       <c r="E64" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F64" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -2416,10 +2416,10 @@
         <v>167</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -2436,7 +2436,7 @@
         <v>170</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -2453,7 +2453,7 @@
         <v>173</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -2467,10 +2467,10 @@
         <v>175</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>